<commit_message>
cleaned up data, added CR, SR and index
</commit_message>
<xml_diff>
--- a/Data/2023_cleaned_events_fixed_V2.xlsx
+++ b/Data/2023_cleaned_events_fixed_V2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2023 Husky Stag- MEN" sheetId="1" state="visible" r:id="rId3"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="363">
   <si>
     <t xml:space="preserve">Event</t>
   </si>
@@ -293,7 +293,7 @@
     <t xml:space="preserve">Nicholas Malshuk</t>
   </si>
   <si>
-    <t xml:space="preserve">Nicholas Oki (+1)</t>
+    <t xml:space="preserve">Nicholas Oki</t>
   </si>
   <si>
     <t xml:space="preserve">Patrick Angelel</t>
@@ -896,9 +896,6 @@
     <t xml:space="preserve">Mason Bernard</t>
   </si>
   <si>
-    <t xml:space="preserve">Nicholas Oki</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nick Long</t>
   </si>
   <si>
@@ -1070,7 +1067,7 @@
     <t xml:space="preserve">Tom van Halm</t>
   </si>
   <si>
-    <t xml:space="preserve">Wesley Boone (+1)</t>
+    <t xml:space="preserve">Wesley Boone</t>
   </si>
   <si>
     <t xml:space="preserve">23 CC Round 1</t>
@@ -1097,7 +1094,7 @@
     <t xml:space="preserve">Owen Otto</t>
   </si>
   <si>
-    <t xml:space="preserve">Pete Higgins (+2)</t>
+    <t xml:space="preserve">Pete Higgins</t>
   </si>
   <si>
     <t xml:space="preserve">Philip Rourke</t>
@@ -1420,8 +1417,8 @@
   </sheetPr>
   <dimension ref="A1:W90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C85" activeCellId="0" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5981,6 +5978,9 @@
       </c>
       <c r="B65" s="3" t="s">
         <v>88</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>-1</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>25</v>
@@ -7836,8 +7836,8 @@
   </sheetPr>
   <dimension ref="A1:W195"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21712,7 +21712,7 @@
   <dimension ref="A1:W195"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35586,8 +35586,8 @@
   </sheetPr>
   <dimension ref="A1:W115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41566,7 +41566,7 @@
         <v>257</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>2</v>
@@ -41637,7 +41637,7 @@
         <v>257</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C86" s="3" t="n">
         <v>5</v>
@@ -41779,7 +41779,7 @@
         <v>257</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C88" s="3" t="n">
         <v>12</v>
@@ -42063,7 +42063,7 @@
         <v>257</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>31</v>
@@ -42347,7 +42347,7 @@
         <v>257</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C96" s="3" t="n">
         <v>11</v>
@@ -42418,7 +42418,7 @@
         <v>257</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C97" s="3" t="n">
         <v>15</v>
@@ -42489,7 +42489,7 @@
         <v>257</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C98" s="3" t="n">
         <v>8</v>
@@ -42702,7 +42702,7 @@
         <v>257</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C101" s="3" t="n">
         <v>21</v>
@@ -42844,7 +42844,7 @@
         <v>257</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C103" s="3" t="n">
         <v>21</v>
@@ -42915,7 +42915,7 @@
         <v>257</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C104" s="3" t="n">
         <v>7</v>
@@ -43128,7 +43128,7 @@
         <v>257</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C107" s="3" t="n">
         <v>7</v>
@@ -43483,7 +43483,7 @@
         <v>257</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C112" s="3" t="n">
         <v>19</v>
@@ -43554,7 +43554,7 @@
         <v>257</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C113" s="3" t="n">
         <v>21</v>
@@ -43625,7 +43625,7 @@
         <v>257</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C114" s="3" t="n">
         <v>21</v>
@@ -43780,8 +43780,8 @@
   </sheetPr>
   <dimension ref="A1:W105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43865,10 +43865,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>304</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>10</v>
@@ -43936,7 +43936,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>115</v>
@@ -44007,7 +44007,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>117</v>
@@ -44078,7 +44078,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -44149,7 +44149,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>121</v>
@@ -44220,7 +44220,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
@@ -44291,7 +44291,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>124</v>
@@ -44362,7 +44362,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>28</v>
@@ -44433,7 +44433,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>127</v>
@@ -44504,7 +44504,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>29</v>
@@ -44575,7 +44575,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>262</v>
@@ -44646,10 +44646,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>9</v>
@@ -44717,7 +44717,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>31</v>
@@ -44788,10 +44788,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>24</v>
@@ -44859,10 +44859,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>22</v>
@@ -44930,7 +44930,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>265</v>
@@ -45001,7 +45001,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>269</v>
@@ -45072,7 +45072,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>138</v>
@@ -45143,10 +45143,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>11</v>
@@ -45214,7 +45214,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>40</v>
@@ -45285,10 +45285,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>8</v>
@@ -45356,7 +45356,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>42</v>
@@ -45427,7 +45427,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>43</v>
@@ -45498,7 +45498,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>153</v>
@@ -45569,7 +45569,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>154</v>
@@ -45640,7 +45640,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>46</v>
@@ -45711,7 +45711,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>48</v>
@@ -45782,7 +45782,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>157</v>
@@ -45853,7 +45853,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>158</v>
@@ -45924,10 +45924,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>0</v>
@@ -45995,7 +45995,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>277</v>
@@ -46066,7 +46066,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>160</v>
@@ -46137,10 +46137,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>12</v>
@@ -46208,10 +46208,10 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>11</v>
@@ -46279,10 +46279,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>19</v>
@@ -46350,7 +46350,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>163</v>
@@ -46421,7 +46421,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>164</v>
@@ -46492,7 +46492,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>52</v>
@@ -46563,7 +46563,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>278</v>
@@ -46634,7 +46634,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>56</v>
@@ -46705,7 +46705,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>280</v>
@@ -46776,7 +46776,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>173</v>
@@ -46847,7 +46847,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>174</v>
@@ -46918,10 +46918,10 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C45" s="3" t="n">
         <v>8</v>
@@ -46989,7 +46989,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>59</v>
@@ -47060,7 +47060,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>281</v>
@@ -47131,7 +47131,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>177</v>
@@ -47202,10 +47202,10 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C49" s="3" t="n">
         <v>11</v>
@@ -47273,7 +47273,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>64</v>
@@ -47344,7 +47344,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>183</v>
@@ -47415,7 +47415,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>69</v>
@@ -47486,7 +47486,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>71</v>
@@ -47557,7 +47557,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>72</v>
@@ -47628,10 +47628,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C55" s="3" t="n">
         <v>19</v>
@@ -47699,7 +47699,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>198</v>
@@ -47770,7 +47770,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>203</v>
@@ -47841,7 +47841,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>204</v>
@@ -47912,7 +47912,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>205</v>
@@ -47983,10 +47983,10 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C60" s="3" t="n">
         <v>21</v>
@@ -48054,7 +48054,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>206</v>
@@ -48125,7 +48125,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>208</v>
@@ -48196,7 +48196,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>79</v>
@@ -48267,7 +48267,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>81</v>
@@ -48338,7 +48338,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>82</v>
@@ -48409,10 +48409,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C66" s="3" t="n">
         <v>20</v>
@@ -48480,7 +48480,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>83</v>
@@ -48551,7 +48551,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>212</v>
@@ -48622,7 +48622,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>213</v>
@@ -48693,10 +48693,10 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C70" s="3" t="n">
         <v>6</v>
@@ -48764,10 +48764,10 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="C71" s="3" t="n">
         <v>0</v>
@@ -48835,10 +48835,10 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C72" s="3" t="n">
         <v>1</v>
@@ -48906,7 +48906,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>216</v>
@@ -48977,10 +48977,10 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C74" s="3" t="n">
         <v>20</v>
@@ -49048,10 +49048,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C75" s="3" t="n">
         <v>19</v>
@@ -49119,7 +49119,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>89</v>
@@ -49190,7 +49190,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>91</v>
@@ -49261,10 +49261,10 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C78" s="3" t="n">
         <v>28</v>
@@ -49332,7 +49332,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>93</v>
@@ -49403,7 +49403,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>94</v>
@@ -49474,7 +49474,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>220</v>
@@ -49545,7 +49545,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>95</v>
@@ -49616,10 +49616,10 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C83" s="3" t="n">
         <v>11</v>
@@ -49687,7 +49687,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>222</v>
@@ -49758,10 +49758,10 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>28</v>
@@ -49829,7 +49829,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>224</v>
@@ -49900,7 +49900,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>225</v>
@@ -49971,7 +49971,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>228</v>
@@ -50042,10 +50042,10 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C89" s="3" t="n">
         <v>20</v>
@@ -50113,10 +50113,10 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C90" s="3" t="n">
         <v>3</v>
@@ -50184,7 +50184,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>236</v>
@@ -50255,10 +50255,10 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>5</v>
@@ -50326,10 +50326,10 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C93" s="3" t="n">
         <v>23</v>
@@ -50397,7 +50397,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>239</v>
@@ -50468,10 +50468,10 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C95" s="3" t="n">
         <v>21</v>
@@ -50539,10 +50539,10 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C96" s="3" t="n">
         <v>10</v>
@@ -50610,10 +50610,10 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C97" s="3" t="n">
         <v>16</v>
@@ -50681,7 +50681,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>103</v>
@@ -50752,7 +50752,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>247</v>
@@ -50823,7 +50823,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>251</v>
@@ -50894,7 +50894,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>108</v>
@@ -50965,7 +50965,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>111</v>
@@ -51036,7 +51036,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>113</v>
@@ -51107,7 +51107,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>253</v>
@@ -51178,10 +51178,10 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C105" s="3" t="n">
         <v>21</v>
@@ -51265,8 +51265,8 @@
   </sheetPr>
   <dimension ref="A1:W81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D84" activeCellId="0" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -51350,10 +51350,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>8</v>
@@ -51421,7 +51421,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>118</v>
@@ -51492,7 +51492,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>26</v>
@@ -51563,7 +51563,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>121</v>
@@ -51634,7 +51634,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>122</v>
@@ -51705,7 +51705,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>27</v>
@@ -51776,7 +51776,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>28</v>
@@ -51847,7 +51847,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>29</v>
@@ -51918,7 +51918,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>263</v>
@@ -51989,7 +51989,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>32</v>
@@ -52060,10 +52060,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>18</v>
@@ -52131,10 +52131,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>3</v>
@@ -52202,7 +52202,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>269</v>
@@ -52273,10 +52273,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>11</v>
@@ -52344,7 +52344,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>40</v>
@@ -52415,10 +52415,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>9</v>
@@ -52486,10 +52486,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>37</v>
@@ -52557,10 +52557,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>11</v>
@@ -52628,10 +52628,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>18</v>
@@ -52699,7 +52699,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>151</v>
@@ -52770,10 +52770,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>20</v>
@@ -52841,7 +52841,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>46</v>
@@ -52912,7 +52912,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>277</v>
@@ -52983,10 +52983,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>12</v>
@@ -53054,10 +53054,10 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>11</v>
@@ -53125,7 +53125,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>52</v>
@@ -53196,7 +53196,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>53</v>
@@ -53267,10 +53267,10 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>15</v>
@@ -53338,7 +53338,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>56</v>
@@ -53409,10 +53409,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>15</v>
@@ -53480,7 +53480,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>174</v>
@@ -53551,7 +53551,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>59</v>
@@ -53622,7 +53622,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>177</v>
@@ -53693,7 +53693,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>180</v>
@@ -53764,7 +53764,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>62</v>
@@ -53835,7 +53835,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>183</v>
@@ -53906,7 +53906,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>69</v>
@@ -53977,10 +53977,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C39" s="3" t="n">
         <v>16</v>
@@ -54048,7 +54048,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>194</v>
@@ -54119,7 +54119,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>198</v>
@@ -54190,7 +54190,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>199</v>
@@ -54261,10 +54261,10 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>20</v>
@@ -54332,7 +54332,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>203</v>
@@ -54403,7 +54403,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>204</v>
@@ -54474,7 +54474,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>205</v>
@@ -54545,10 +54545,10 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C47" s="3" t="n">
         <v>20</v>
@@ -54616,7 +54616,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>206</v>
@@ -54687,7 +54687,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>207</v>
@@ -54758,7 +54758,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>80</v>
@@ -54829,7 +54829,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>82</v>
@@ -54900,10 +54900,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C52" s="3" t="n">
         <v>22</v>
@@ -54971,7 +54971,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>83</v>
@@ -55042,10 +55042,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C54" s="3" t="n">
         <v>20</v>
@@ -55113,10 +55113,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C55" s="3" t="n">
         <v>6</v>
@@ -55184,7 +55184,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>212</v>
@@ -55255,7 +55255,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>213</v>
@@ -55326,7 +55326,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>86</v>
@@ -55397,10 +55397,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="C59" s="3" t="n">
         <v>2</v>
@@ -55468,7 +55468,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>89</v>
@@ -55539,10 +55539,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C61" s="3" t="n">
         <v>29</v>
@@ -55610,7 +55610,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>94</v>
@@ -55681,7 +55681,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>220</v>
@@ -55752,7 +55752,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>98</v>
@@ -55823,7 +55823,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>99</v>
@@ -55894,10 +55894,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C66" s="3" t="n">
         <v>28</v>
@@ -55965,7 +55965,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>224</v>
@@ -56036,7 +56036,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>228</v>
@@ -56107,7 +56107,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>235</v>
@@ -56178,7 +56178,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>239</v>
@@ -56249,10 +56249,10 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C71" s="3" t="n">
         <v>20</v>
@@ -56320,7 +56320,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>103</v>
@@ -56391,7 +56391,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>247</v>
@@ -56462,7 +56462,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>251</v>
@@ -56533,10 +56533,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C75" s="3" t="n">
         <v>8</v>
@@ -56604,7 +56604,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>108</v>
@@ -56675,7 +56675,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>109</v>
@@ -56746,7 +56746,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>111</v>
@@ -56817,7 +56817,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>113</v>
@@ -56888,10 +56888,13 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>-1</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>25</v>
@@ -56956,10 +56959,10 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C81" s="3" t="n">
         <v>21</v>
@@ -57044,7 +57047,7 @@
   <dimension ref="A1:W101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+      <selection pane="topLeft" activeCell="B77" activeCellId="0" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -57127,7 +57130,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>24</v>
@@ -57198,7 +57201,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>118</v>
@@ -57269,7 +57272,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>119</v>
@@ -57340,7 +57343,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>26</v>
@@ -57411,7 +57414,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>121</v>
@@ -57482,7 +57485,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>124</v>
@@ -57553,7 +57556,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>29</v>
@@ -57624,7 +57627,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>30</v>
@@ -57695,7 +57698,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>129</v>
@@ -57766,7 +57769,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>130</v>
@@ -57837,10 +57840,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>7</v>
@@ -57908,7 +57911,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>134</v>
@@ -57979,7 +57982,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>135</v>
@@ -58050,7 +58053,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>137</v>
@@ -58121,7 +58124,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>37</v>
@@ -58192,7 +58195,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>139</v>
@@ -58263,10 +58266,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>3</v>
@@ -58334,7 +58337,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>141</v>
@@ -58405,7 +58408,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>40</v>
@@ -58476,7 +58479,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>144</v>
@@ -58547,7 +58550,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>43</v>
@@ -58618,7 +58621,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>273</v>
@@ -58689,7 +58692,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>151</v>
@@ -58760,7 +58763,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>155</v>
@@ -58831,7 +58834,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>47</v>
@@ -58902,10 +58905,10 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>29</v>
@@ -58973,7 +58976,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>158</v>
@@ -59044,7 +59047,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>159</v>
@@ -59115,10 +59118,10 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>0</v>
@@ -59186,7 +59189,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>50</v>
@@ -59257,7 +59260,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>162</v>
@@ -59328,7 +59331,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>163</v>
@@ -59399,7 +59402,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>52</v>
@@ -59470,7 +59473,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>278</v>
@@ -59541,10 +59544,10 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>0</v>
@@ -59612,7 +59615,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>53</v>
@@ -59683,7 +59686,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>55</v>
@@ -59754,7 +59757,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>165</v>
@@ -59825,7 +59828,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>167</v>
@@ -59896,10 +59899,10 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C41" s="3" t="n">
         <v>27</v>
@@ -59967,7 +59970,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>56</v>
@@ -60038,7 +60041,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>280</v>
@@ -60109,7 +60112,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>174</v>
@@ -60180,7 +60183,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>59</v>
@@ -60251,7 +60254,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>177</v>
@@ -60322,7 +60325,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>61</v>
@@ -60393,7 +60396,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>183</v>
@@ -60464,7 +60467,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>66</v>
@@ -60535,7 +60538,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>184</v>
@@ -60606,7 +60609,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>185</v>
@@ -60677,7 +60680,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>186</v>
@@ -60748,7 +60751,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>188</v>
@@ -60819,7 +60822,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>69</v>
@@ -60890,7 +60893,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>191</v>
@@ -60961,7 +60964,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>72</v>
@@ -61032,7 +61035,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>74</v>
@@ -61103,7 +61106,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>199</v>
@@ -61174,7 +61177,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>203</v>
@@ -61245,7 +61248,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>204</v>
@@ -61316,7 +61319,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>205</v>
@@ -61387,7 +61390,7 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>206</v>
@@ -61458,7 +61461,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>207</v>
@@ -61529,7 +61532,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>79</v>
@@ -61600,7 +61603,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>80</v>
@@ -61671,10 +61674,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C66" s="3" t="n">
         <v>25</v>
@@ -61742,7 +61745,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>83</v>
@@ -61813,7 +61816,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>210</v>
@@ -61884,7 +61887,7 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>212</v>
@@ -61955,7 +61958,7 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>213</v>
@@ -62026,10 +62029,10 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="C71" s="3" t="n">
         <v>5</v>
@@ -62097,7 +62100,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>216</v>
@@ -62168,10 +62171,10 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C73" s="3" t="n">
         <v>14</v>
@@ -62239,10 +62242,10 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C74" s="3" t="n">
         <v>2</v>
@@ -62310,7 +62313,7 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>89</v>
@@ -62381,7 +62384,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>93</v>
@@ -62452,10 +62455,13 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>-2</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>25</v>
@@ -62520,7 +62526,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>220</v>
@@ -62591,10 +62597,10 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C79" s="3" t="n">
         <v>17</v>
@@ -62662,7 +62668,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>97</v>
@@ -62733,7 +62739,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>224</v>
@@ -62804,7 +62810,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>226</v>
@@ -62875,7 +62881,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>228</v>
@@ -62946,10 +62952,10 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C84" s="3" t="n">
         <v>10</v>
@@ -63017,7 +63023,7 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>231</v>
@@ -63088,7 +63094,7 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>100</v>
@@ -63159,7 +63165,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>236</v>
@@ -63230,10 +63236,10 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C88" s="3" t="n">
         <v>13</v>
@@ -63301,7 +63307,7 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>239</v>
@@ -63372,10 +63378,10 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C90" s="3" t="n">
         <v>20</v>
@@ -63443,10 +63449,10 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C91" s="3" t="n">
         <v>12</v>
@@ -63514,7 +63520,7 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>103</v>
@@ -63585,7 +63591,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>247</v>
@@ -63656,10 +63662,10 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C94" s="3" t="n">
         <v>8</v>
@@ -63727,10 +63733,10 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C95" s="3" t="n">
         <v>2</v>
@@ -63798,7 +63804,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>106</v>
@@ -63869,7 +63875,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>251</v>
@@ -63940,10 +63946,10 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C98" s="3" t="n">
         <v>17</v>
@@ -64011,7 +64017,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>108</v>
@@ -64082,7 +64088,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>111</v>
@@ -64153,7 +64159,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>253</v>
@@ -64240,8 +64246,8 @@
   </sheetPr>
   <dimension ref="A1:W95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A95"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B74" activeCellId="0" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -64325,7 +64331,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>24</v>
@@ -64396,7 +64402,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>119</v>
@@ -64467,7 +64473,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>26</v>
@@ -64538,7 +64544,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>121</v>
@@ -64609,7 +64615,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>124</v>
@@ -64680,7 +64686,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>29</v>
@@ -64751,7 +64757,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>30</v>
@@ -64822,7 +64828,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>129</v>
@@ -64893,7 +64899,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>130</v>
@@ -64964,10 +64970,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>7</v>
@@ -65035,7 +65041,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>134</v>
@@ -65106,7 +65112,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>135</v>
@@ -65177,7 +65183,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>137</v>
@@ -65248,7 +65254,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>37</v>
@@ -65319,7 +65325,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>139</v>
@@ -65390,10 +65396,10 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>3</v>
@@ -65461,7 +65467,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>141</v>
@@ -65532,7 +65538,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>40</v>
@@ -65603,7 +65609,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>144</v>
@@ -65674,7 +65680,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>273</v>
@@ -65745,7 +65751,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>151</v>
@@ -65816,7 +65822,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>155</v>
@@ -65887,7 +65893,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>47</v>
@@ -65958,10 +65964,10 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>29</v>
@@ -66029,7 +66035,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>158</v>
@@ -66100,7 +66106,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>159</v>
@@ -66171,10 +66177,10 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>0</v>
@@ -66242,7 +66248,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>50</v>
@@ -66313,7 +66319,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>162</v>
@@ -66384,7 +66390,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>163</v>
@@ -66455,7 +66461,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>52</v>
@@ -66526,7 +66532,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>278</v>
@@ -66597,10 +66603,10 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>0</v>
@@ -66668,7 +66674,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>53</v>
@@ -66739,7 +66745,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>55</v>
@@ -66810,7 +66816,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>165</v>
@@ -66881,7 +66887,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>167</v>
@@ -66952,10 +66958,10 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C39" s="3" t="n">
         <v>27</v>
@@ -67023,7 +67029,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>56</v>
@@ -67094,7 +67100,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>280</v>
@@ -67165,7 +67171,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>174</v>
@@ -67236,7 +67242,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>59</v>
@@ -67307,7 +67313,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>61</v>
@@ -67378,7 +67384,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>183</v>
@@ -67449,7 +67455,7 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>66</v>
@@ -67520,7 +67526,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>184</v>
@@ -67591,7 +67597,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>185</v>
@@ -67662,7 +67668,7 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>186</v>
@@ -67733,7 +67739,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>188</v>
@@ -67804,7 +67810,7 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>69</v>
@@ -67875,7 +67881,7 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>191</v>
@@ -67946,7 +67952,7 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>72</v>
@@ -68017,7 +68023,7 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>74</v>
@@ -68088,7 +68094,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>199</v>
@@ -68159,7 +68165,7 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>204</v>
@@ -68230,7 +68236,7 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>205</v>
@@ -68301,7 +68307,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>206</v>
@@ -68372,7 +68378,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>207</v>
@@ -68443,7 +68449,7 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>79</v>
@@ -68514,7 +68520,7 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>80</v>
@@ -68585,10 +68591,10 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C62" s="3" t="n">
         <v>25</v>
@@ -68656,7 +68662,7 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>83</v>
@@ -68727,7 +68733,7 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>210</v>
@@ -68798,7 +68804,7 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>212</v>
@@ -68869,7 +68875,7 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>213</v>
@@ -68940,10 +68946,10 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="C67" s="3" t="n">
         <v>5</v>
@@ -69011,7 +69017,7 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>216</v>
@@ -69082,10 +69088,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C69" s="3" t="n">
         <v>14</v>
@@ -69153,10 +69159,10 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C70" s="3" t="n">
         <v>2</v>
@@ -69224,7 +69230,7 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>89</v>
@@ -69295,7 +69301,7 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>93</v>
@@ -69366,10 +69372,13 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>-2</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>25</v>
@@ -69434,7 +69443,7 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>220</v>
@@ -69505,10 +69514,10 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C75" s="3" t="n">
         <v>17</v>
@@ -69576,7 +69585,7 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>97</v>
@@ -69647,7 +69656,7 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>224</v>
@@ -69718,7 +69727,7 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>226</v>
@@ -69789,7 +69798,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>228</v>
@@ -69860,10 +69869,10 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C80" s="3" t="n">
         <v>10</v>
@@ -69931,7 +69940,7 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>231</v>
@@ -70002,7 +70011,7 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>100</v>
@@ -70073,7 +70082,7 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>236</v>
@@ -70144,10 +70153,10 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C84" s="3" t="n">
         <v>13</v>
@@ -70215,10 +70224,10 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>20</v>
@@ -70286,10 +70295,10 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C86" s="3" t="n">
         <v>12</v>
@@ -70357,7 +70366,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>103</v>
@@ -70428,7 +70437,7 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>247</v>
@@ -70499,10 +70508,10 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C89" s="3" t="n">
         <v>2</v>
@@ -70570,7 +70579,7 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>106</v>
@@ -70641,7 +70650,7 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>251</v>
@@ -70712,10 +70721,10 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>17</v>
@@ -70783,7 +70792,7 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>108</v>
@@ -70854,7 +70863,7 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>111</v>
@@ -70925,7 +70934,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>253</v>

</xml_diff>